<commit_message>
feat(converter): add working export-to-template pipeline with file watching and rename logic
- Implemented watcher to detect incoming export files
- Added GUI input for prefix/year/tag selection
- Added Excel converter and template generator
- Added atomic file write and safe move to excel_templates/
- Added processed-folder workflow for completed files
- Cleaned up .gitignore according to project structure
</commit_message>
<xml_diff>
--- a/excel_templates/processed/EDS-2025-RR.xlsx
+++ b/excel_templates/processed/EDS-2025-RR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://edsth-my.sharepoint.com/personal/piyaphon_w_eds_co_th/Documents/Desktop/New folder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{5A44E851-D78A-4EF8-A7DE-F80C3D7D6DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{57638E3B-E880-44E5-939D-BE7E0E382909}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{5A44E851-D78A-4EF8-A7DE-F80C3D7D6DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{373D0693-ED22-4640-84BB-F4BEB262E250}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-2535" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,14 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
   <si>
-    <t>MBK</t>
-  </si>
-  <si>
     <t>026959000</t>
   </si>
   <si>
@@ -57,16 +54,25 @@
     <t>UnitCost</t>
   </si>
   <si>
-    <t>01/10/68</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1.00 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 4,350.00 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 22,495.82 </t>
+    <t>BKK</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>5,014.85</t>
+  </si>
+  <si>
+    <t>FPR</t>
+  </si>
+  <si>
+    <t>935.97</t>
+  </si>
+  <si>
+    <t>011125</t>
+  </si>
+  <si>
+    <t>111125</t>
   </si>
 </sst>
 </file>
@@ -407,7 +413,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -415,7 +421,7 @@
     <col min="1" max="1" width="10.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
@@ -424,68 +430,68 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2">
+        <v>6500128102</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2">
-        <v>6500118096</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="D3">
+        <v>6500128103</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>6500118097</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>13</v>

</xml_diff>